<commit_message>
Completed DS 775 HW 5
</commit_message>
<xml_diff>
--- a/wk5/HW_5_Isaacson.xlsx
+++ b/wk5/HW_5_Isaacson.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myscripts\school\ds775\wk5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="897" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8565" windowHeight="7965" tabRatio="897" firstSheet="6" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="4.7-6 Sensitivity Report" sheetId="6" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <sheet name="7.3-7" sheetId="38" r:id="rId9"/>
     <sheet name="7.4-4" sheetId="40" r:id="rId10"/>
     <sheet name="7.5-1" sheetId="42" r:id="rId11"/>
+    <sheet name="7.5-4" sheetId="43" r:id="rId12"/>
+    <sheet name="7.6-1" sheetId="44" r:id="rId13"/>
+    <sheet name="7.6-3" sheetId="45" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="AgentsPerShift">'7.3-7'!$D$18:$H$18</definedName>
@@ -41,6 +44,7 @@
     <definedName name="coin_presolve1" localSheetId="6" hidden="1">1</definedName>
     <definedName name="coin_primaltol" localSheetId="4" hidden="1">0.0000001</definedName>
     <definedName name="coin_primaltol" localSheetId="6" hidden="1">0.0000001</definedName>
+    <definedName name="constraint" localSheetId="11">#REF!</definedName>
     <definedName name="constraint">#REF!</definedName>
     <definedName name="DailyCostPerAgent">'7.3-7'!$D$5:$H$5</definedName>
     <definedName name="grb_async_callbacks" localSheetId="1" hidden="1">1</definedName>
@@ -138,7 +142,9 @@
     <definedName name="gurobi_qp" localSheetId="6" hidden="1">0</definedName>
     <definedName name="MinimunAgentsNeeded">'7.3-7'!$K$7:$K$16</definedName>
     <definedName name="MinimunAgentsPerTimePeriod">'7.3-7'!$K$7:$K$16</definedName>
+    <definedName name="objective" localSheetId="11">#REF!</definedName>
     <definedName name="objective">#REF!</definedName>
+    <definedName name="out" localSheetId="11">#REF!</definedName>
     <definedName name="out">#REF!</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'4.7-6'!$C$9:$F$9</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'7.3-4'!$C$9:$D$9</definedName>
@@ -146,6 +152,9 @@
     <definedName name="solver_adj" localSheetId="8" hidden="1">'7.3-7'!$D$18:$H$18</definedName>
     <definedName name="solver_adj" localSheetId="9" hidden="1">'7.4-4'!$C$33:$E$33</definedName>
     <definedName name="solver_adj" localSheetId="10" hidden="1">'7.5-1'!$C$9:$D$9</definedName>
+    <definedName name="solver_adj" localSheetId="11" hidden="1">'7.5-4'!$C$9:$E$9</definedName>
+    <definedName name="solver_adj" localSheetId="12" hidden="1">'7.6-1'!$C$11:$E$11</definedName>
+    <definedName name="solver_adj" localSheetId="13" hidden="1">'7.6-3'!$D$14:$G$14</definedName>
     <definedName name="solver_adj_ob" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_adj_ob" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_adj_ob" localSheetId="6" hidden="1">1</definedName>
@@ -183,6 +192,9 @@
     <definedName name="solver_cvg" localSheetId="8" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="9" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="10" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="11" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="12" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="13" hidden="1">0.0001</definedName>
     <definedName name="solver_dia" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_dia" localSheetId="4" hidden="1">5</definedName>
     <definedName name="solver_dia" localSheetId="6" hidden="1">5</definedName>
@@ -192,18 +204,27 @@
     <definedName name="solver_drv" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="12" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="13" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">6</definedName>
     <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="12" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="13" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="12" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="13" hidden="1">1</definedName>
     <definedName name="solver_eval" hidden="1">0</definedName>
     <definedName name="solver_iao" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_iao" localSheetId="4" hidden="1">0</definedName>
@@ -223,6 +244,9 @@
     <definedName name="solver_itr" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="10" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="12" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="13" hidden="1">2147483647</definedName>
     <definedName name="solver_kiv" localSheetId="4" hidden="1">2E+30</definedName>
     <definedName name="solver_kiv" localSheetId="6" hidden="1">2E+30</definedName>
     <definedName name="solver_lhs_ob1" localSheetId="1" hidden="1">0</definedName>
@@ -235,8 +259,12 @@
     <definedName name="solver_lhs1" localSheetId="8" hidden="1">'7.3-7'!$I$7:$I$16</definedName>
     <definedName name="solver_lhs1" localSheetId="9" hidden="1">'7.4-4'!$F$29</definedName>
     <definedName name="solver_lhs1" localSheetId="10" hidden="1">'7.5-1'!$E$5:$E$7</definedName>
+    <definedName name="solver_lhs1" localSheetId="11" hidden="1">'7.5-4'!$F$5:$F$7</definedName>
+    <definedName name="solver_lhs1" localSheetId="12" hidden="1">'7.6-1'!$F$5:$F$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="13" hidden="1">'7.6-3'!$H$12</definedName>
     <definedName name="solver_lhs2" localSheetId="6" hidden="1">'7.3-5'!$C$9</definedName>
     <definedName name="solver_lhs2" localSheetId="9" hidden="1">'7.4-4'!$F$30</definedName>
+    <definedName name="solver_lhs2" localSheetId="13" hidden="1">'7.6-3'!$H$8:$H$11</definedName>
     <definedName name="solver_lhs3" localSheetId="9" hidden="1">'7.4-4'!$F$31</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="4" hidden="1">2</definedName>
@@ -250,12 +278,18 @@
     <definedName name="solver_mip" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="10" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="12" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="13" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="8" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="9" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="10" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="11" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="12" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="13" hidden="1">30</definedName>
     <definedName name="solver_mod" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_mod" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_mod" localSheetId="6" hidden="1">3</definedName>
@@ -265,24 +299,36 @@
     <definedName name="solver_mrt" localSheetId="8" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="9" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="10" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="11" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="12" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="13" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="12" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="13" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="12" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="13" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="10" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="12" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="13" hidden="1">2147483647</definedName>
     <definedName name="solver_nopt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nopt" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_ntr" localSheetId="1" hidden="1">0</definedName>
@@ -295,12 +341,18 @@
     <definedName name="solver_num" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="9" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="12" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="13" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="12" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="13" hidden="1">1</definedName>
     <definedName name="solver_obc" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_obc" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_obc" localSheetId="6" hidden="1">0</definedName>
@@ -313,6 +365,9 @@
     <definedName name="solver_opt" localSheetId="8" hidden="1">'7.3-7'!$K$18</definedName>
     <definedName name="solver_opt" localSheetId="9" hidden="1">'7.4-4'!$H$33</definedName>
     <definedName name="solver_opt" localSheetId="10" hidden="1">'7.5-1'!$G$9</definedName>
+    <definedName name="solver_opt" localSheetId="11" hidden="1">'7.5-4'!$H$9</definedName>
+    <definedName name="solver_opt" localSheetId="12" hidden="1">'7.6-1'!$H$11</definedName>
+    <definedName name="solver_opt" localSheetId="13" hidden="1">'7.6-3'!$J$14</definedName>
     <definedName name="solver_opt_ob" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt_ob" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_opt_ob" localSheetId="6" hidden="1">1</definedName>
@@ -322,6 +377,9 @@
     <definedName name="solver_pre" localSheetId="8" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="9" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="10" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="11" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="12" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="13" hidden="1">0.000001</definedName>
     <definedName name="solver_psi" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_psi" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_psi" localSheetId="6" hidden="1">0</definedName>
@@ -331,6 +389,9 @@
     <definedName name="solver_rbv" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="12" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="13" hidden="1">2</definedName>
     <definedName name="solver_rdp" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rdp" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_rdp" localSheetId="6" hidden="1">0</definedName>
@@ -344,8 +405,12 @@
     <definedName name="solver_rel1" localSheetId="8" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="12" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="13" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="9" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="13" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_rep" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rep" localSheetId="4" hidden="1">0</definedName>
@@ -356,8 +421,12 @@
     <definedName name="solver_rhs1" localSheetId="8" hidden="1">MinimunAgentsNeeded</definedName>
     <definedName name="solver_rhs1" localSheetId="9" hidden="1">'7.4-4'!$H$29</definedName>
     <definedName name="solver_rhs1" localSheetId="10" hidden="1">'7.5-1'!$G$5:$G$7</definedName>
+    <definedName name="solver_rhs1" localSheetId="11" hidden="1">'7.5-4'!$H$5:$H$7</definedName>
+    <definedName name="solver_rhs1" localSheetId="12" hidden="1">'7.6-1'!$H$5:$H$9</definedName>
+    <definedName name="solver_rhs1" localSheetId="13" hidden="1">'7.6-3'!$J$12</definedName>
     <definedName name="solver_rhs2" localSheetId="6" hidden="1">'7.3-5'!$C$11</definedName>
     <definedName name="solver_rhs2" localSheetId="9" hidden="1">'7.4-4'!$H$30</definedName>
+    <definedName name="solver_rhs2" localSheetId="13" hidden="1">'7.6-3'!$J$8:$J$11</definedName>
     <definedName name="solver_rhs3" localSheetId="9" hidden="1">'7.4-4'!$H$31</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">0</definedName>
@@ -365,12 +434,18 @@
     <definedName name="solver_rlx" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="12" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="13" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="9" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="10" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="12" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="13" hidden="1">0</definedName>
     <definedName name="solver_rsmp" hidden="1">2</definedName>
     <definedName name="solver_rtr" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rtr" localSheetId="4" hidden="1">0</definedName>
@@ -388,6 +463,9 @@
     <definedName name="solver_scl" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="12" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="13" hidden="1">2</definedName>
     <definedName name="solver_seed" hidden="1">0</definedName>
     <definedName name="solver_sel" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sel" localSheetId="4" hidden="1">1</definedName>
@@ -398,6 +476,9 @@
     <definedName name="solver_sho" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="12" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="13" hidden="1">2</definedName>
     <definedName name="solver_slv" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_slv" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_slv" localSheetId="6" hidden="1">0</definedName>
@@ -416,24 +497,36 @@
     <definedName name="solver_ssz" localSheetId="8" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="9" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="10" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="11" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="12" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="13" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="10" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="12" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="13" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="8" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="9" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="10" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="11" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="12" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="13" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="12" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="13" hidden="1">1</definedName>
     <definedName name="solver_umod" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_umod" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_umod" localSheetId="6" hidden="1">1</definedName>
@@ -451,6 +544,9 @@
     <definedName name="solver_val" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="9" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="10" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="12" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="13" hidden="1">0</definedName>
     <definedName name="solver_var" localSheetId="1" hidden="1">" "</definedName>
     <definedName name="solver_var" localSheetId="4" hidden="1">" "</definedName>
     <definedName name="solver_var" localSheetId="6" hidden="1">" "</definedName>
@@ -460,6 +556,9 @@
     <definedName name="solver_ver" localSheetId="8" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="9" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="10" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="11" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="12" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="13" hidden="1">3</definedName>
     <definedName name="solver_vir" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_vir" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_vir" localSheetId="6" hidden="1">1</definedName>
@@ -470,12 +569,14 @@
     <definedName name="solver_vst" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_vst" localSheetId="6" hidden="1">0</definedName>
     <definedName name="TotalCost">'7.3-7'!$K$18</definedName>
+    <definedName name="var" localSheetId="11">#REF!</definedName>
     <definedName name="var">#REF!</definedName>
+    <definedName name="variable" localSheetId="11">#REF!</definedName>
     <definedName name="variable">#REF!</definedName>
   </definedNames>
   <calcPr calcId="171027" calcOnSave="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId15"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -486,7 +587,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="95">
   <si>
     <t>&gt;=</t>
   </si>
@@ -750,6 +851,27 @@
   </si>
   <si>
     <t>7.5-1</t>
+  </si>
+  <si>
+    <t>7.5-4</t>
+  </si>
+  <si>
+    <t>7.6-1</t>
+  </si>
+  <si>
+    <t>.50(3x1 + 5x21) + 0.50(3x1 + x22)</t>
+  </si>
+  <si>
+    <t>3x1 + 2.50x21 + 0.50x22</t>
+  </si>
+  <si>
+    <t>7.6-3</t>
+  </si>
+  <si>
+    <t>0.5*x1 + 0.25(2*x21) + 0.25(0.2*x22) + 0.50(0*x23) -40</t>
+  </si>
+  <si>
+    <t>0.5*x1 + 0.50x21 + 0.005x22 + 0x23</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1256,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -1177,9 +1299,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1266,6 +1385,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
@@ -1521,6 +1644,11 @@
     <dataField name=" $G$9 " fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
 </pivotTableDefinition>
 </file>
 
@@ -1828,39 +1956,39 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="2" max="2" width="4.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.86328125" customWidth="1"/>
-    <col min="8" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
@@ -1879,7 +2007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
@@ -1902,7 +2030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>37</v>
       </c>
@@ -1913,7 +2041,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
@@ -1936,7 +2064,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>29</v>
       </c>
@@ -1959,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
@@ -1982,7 +2110,7 @@
         <v>1.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.65" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>33</v>
       </c>
@@ -2005,7 +2133,7 @@
         <v>1.3333333333333335</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -2014,12 +2142,12 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
@@ -2038,7 +2166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
@@ -2061,7 +2189,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
@@ -2082,7 +2210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>36</v>
       </c>
@@ -2116,426 +2244,426 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C3" s="40" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="42"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C4" s="43"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="45"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C5" s="43" t="s">
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="42"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44" t="s">
+      <c r="F5" s="43"/>
+      <c r="G5" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="44" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C6" s="43" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="45" t="s">
+      <c r="F6" s="43"/>
+      <c r="G6" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="44" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C7" s="43" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44" t="s">
+      <c r="F7" s="43"/>
+      <c r="G7" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="44" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C8" s="43"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="45"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C9" s="46"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="48"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C11" s="49">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="42"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="44"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="45"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="47"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="48">
         <v>5</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C12" s="52"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="54"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C13" s="52" t="s">
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="50"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="51"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="53"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="53">
+      <c r="D13" s="52">
         <v>-3</v>
       </c>
-      <c r="E13" s="53">
+      <c r="E13" s="52">
         <v>2</v>
       </c>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53" t="s">
+      <c r="F13" s="52"/>
+      <c r="G13" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="54" t="s">
+      <c r="H13" s="53" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C14" s="52">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="51">
         <v>3</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="53">
+      <c r="E14" s="52">
         <v>1</v>
       </c>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="54" t="s">
+      <c r="F14" s="52"/>
+      <c r="G14" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="53" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C15" s="52">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="51">
         <v>2</v>
       </c>
-      <c r="D15" s="53">
+      <c r="D15" s="52">
         <v>-4</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53" t="s">
+      <c r="F15" s="52"/>
+      <c r="G15" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="54">
+      <c r="H15" s="53">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="45"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="48"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C19" s="55">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="42"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="44"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="45"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="47"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="54">
         <v>5</v>
       </c>
-      <c r="D19" s="65">
+      <c r="D19" s="64">
         <v>-8</v>
       </c>
-      <c r="E19" s="65">
+      <c r="E19" s="64">
         <v>4</v>
       </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="57"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C20" s="58"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="60"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C21" s="64">
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="56"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="57"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="59"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="63">
         <v>4</v>
       </c>
-      <c r="D21" s="59">
+      <c r="D21" s="58">
         <v>-3</v>
       </c>
-      <c r="E21" s="59">
+      <c r="E21" s="58">
         <v>2</v>
       </c>
-      <c r="F21" s="59">
+      <c r="F21" s="58">
         <f>SUMPRODUCT(C21:E21,$C$25:$E$25)</f>
         <v>30</v>
       </c>
-      <c r="G21" s="59" t="s">
+      <c r="G21" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="66">
+      <c r="H21" s="65">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C22" s="58">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="57">
         <v>3</v>
       </c>
-      <c r="D22" s="63">
+      <c r="D22" s="62">
         <v>-1</v>
       </c>
-      <c r="E22" s="59">
+      <c r="E22" s="58">
         <v>1</v>
       </c>
-      <c r="F22" s="59">
+      <c r="F22" s="58">
         <f t="shared" ref="F22:F23" si="0">SUMPRODUCT(C22:E22,$C$25:$E$25)</f>
         <v>21.25</v>
       </c>
-      <c r="G22" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="H22" s="66">
+      <c r="G22" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="65">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C23" s="58">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="57">
         <v>2</v>
       </c>
-      <c r="D23" s="59">
+      <c r="D23" s="58">
         <v>-4</v>
       </c>
-      <c r="E23" s="63">
+      <c r="E23" s="62">
         <v>3</v>
       </c>
-      <c r="F23" s="59">
+      <c r="F23" s="58">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G23" s="59" t="s">
+      <c r="G23" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="60">
+      <c r="H23" s="59">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C24" s="58"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="60"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C25" s="61">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="59"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="60">
         <v>6.25</v>
       </c>
-      <c r="D25" s="62">
-        <v>0</v>
-      </c>
-      <c r="E25" s="62">
+      <c r="D25" s="61">
+        <v>0</v>
+      </c>
+      <c r="E25" s="61">
         <v>2.5</v>
       </c>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="68">
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="67">
         <f>SUMPRODUCT(C19:E19,C25:E25)</f>
         <v>41.25</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C27" s="55">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="54">
         <v>5</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="64">
         <v>-9</v>
       </c>
-      <c r="E27" s="65">
+      <c r="E27" s="64">
         <v>3</v>
       </c>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="57"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C28" s="58"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="60"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C29" s="64">
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="56"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="57"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="59"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="63">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D29" s="59">
+      <c r="D29" s="58">
         <v>-3</v>
       </c>
-      <c r="E29" s="59">
+      <c r="E29" s="58">
         <v>2</v>
       </c>
-      <c r="F29" s="59">
+      <c r="F29" s="58">
         <f>SUMPRODUCT(C29:E29,$C$33:$E$33)</f>
         <v>27</v>
       </c>
-      <c r="G29" s="59" t="s">
+      <c r="G29" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="66">
+      <c r="H29" s="65">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C30" s="58">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="57">
         <v>3</v>
       </c>
-      <c r="D30" s="63">
+      <c r="D30" s="62">
         <v>-1.4</v>
       </c>
-      <c r="E30" s="59">
+      <c r="E30" s="58">
         <v>1</v>
       </c>
-      <c r="F30" s="59">
+      <c r="F30" s="58">
         <f t="shared" ref="F30:F31" si="1">SUMPRODUCT(C30:E30,$C$33:$E$33)</f>
         <v>19</v>
       </c>
-      <c r="G30" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="H30" s="66">
+      <c r="G30" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="65">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C31" s="58">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="57">
         <v>2</v>
       </c>
-      <c r="D31" s="59">
+      <c r="D31" s="58">
         <v>-4</v>
       </c>
-      <c r="E31" s="63">
+      <c r="E31" s="62">
         <v>3.5</v>
       </c>
-      <c r="F31" s="59">
+      <c r="F31" s="58">
         <f t="shared" si="1"/>
         <v>9.8591549295774517</v>
       </c>
-      <c r="G31" s="59" t="s">
+      <c r="G31" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="H31" s="60">
+      <c r="H31" s="59">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="60"/>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="C33" s="61">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="59"/>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="60">
         <v>6.7605633802816918</v>
       </c>
-      <c r="D33" s="62">
+      <c r="D33" s="61">
         <v>0.91549295774648287</v>
       </c>
-      <c r="E33" s="62">
-        <v>0</v>
-      </c>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="68">
+      <c r="E33" s="61">
+        <v>0</v>
+      </c>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="67">
         <f>SUMPRODUCT(C27:E27,C33:E33)</f>
         <v>25.563380281690115</v>
       </c>
-      <c r="I33" s="67">
+      <c r="I33" s="66">
         <f>(H33-H25)/H25</f>
         <v>-0.38028169014084567</v>
       </c>
@@ -2549,28 +2677,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" customWidth="1"/>
-    <col min="2" max="2" width="3.796875" customWidth="1"/>
-    <col min="3" max="3" width="4.86328125" customWidth="1"/>
-    <col min="4" max="4" width="4.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" customWidth="1"/>
-    <col min="6" max="6" width="2.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" s="1">
         <v>3</v>
       </c>
@@ -2578,7 +2706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -2596,7 +2724,7 @@
         <v>3.77</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>0</v>
       </c>
@@ -2614,7 +2742,7 @@
         <v>11.42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -2632,16 +2760,487 @@
         <v>16.84</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C9" s="29">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="28">
         <v>1.8066666666666666</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>5.71</v>
       </c>
       <c r="G9" s="3">
         <f>SUMPRODUCT(C3:D3,C9:D9)</f>
         <v>33.97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+    <col min="4" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="2.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f>SUMPRODUCT(C5:E5,$C$9:$E$9)</f>
+        <v>84.12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5">
+        <v>84.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F7" si="0">SUMPRODUCT(C6:E6,$C$9:$E$9)</f>
+        <v>140.16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6">
+        <v>140.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>168.47999999999996</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7">
+        <v>168.48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="28">
+        <v>7.0200000000000031</v>
+      </c>
+      <c r="D9" s="28">
+        <v>21.977142857142859</v>
+      </c>
+      <c r="E9" s="28">
+        <v>19.105714285714278</v>
+      </c>
+      <c r="H9" s="3">
+        <f>SUMPRODUCT(C3:E3,C9:E9)</f>
+        <v>1277.3571428571429</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="1.5703125" customWidth="1"/>
+    <col min="3" max="8" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>SUMPRODUCT(C5:E5,$C$11:$E$11)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F9" si="0">SUMPRODUCT(C6:E6,$C$11:$E$11)</f>
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="28">
+        <v>2</v>
+      </c>
+      <c r="D11" s="28">
+        <v>6</v>
+      </c>
+      <c r="E11" s="28">
+        <v>2</v>
+      </c>
+      <c r="H11" s="69">
+        <f>SUMPRODUCT(C3:E3,C11:E11)</f>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="3" width="1.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>SUMPRODUCT(D8:G8,$D$14:$G$14)</f>
+        <v>100</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9">
+        <f t="shared" ref="H9:H12" si="0">SUMPRODUCT(D9:G9,$D$14:$G$14)</f>
+        <v>100</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="28">
+        <v>5</v>
+      </c>
+      <c r="E14" s="28">
+        <v>95</v>
+      </c>
+      <c r="F14" s="28">
+        <v>95</v>
+      </c>
+      <c r="G14" s="28">
+        <v>0</v>
+      </c>
+      <c r="I14" s="28">
+        <v>40</v>
+      </c>
+      <c r="J14" s="3">
+        <f>SUMPRODUCT(D6:G6,D14:G14)-40</f>
+        <v>10.475000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2658,22 +3257,22 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -2687,7 +3286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -2704,16 +3303,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -2740,7 +3339,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
@@ -2767,7 +3366,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -2805,38 +3404,38 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="2" max="2" width="4.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.86328125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14" t="s">
@@ -2855,7 +3454,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
@@ -2878,7 +3477,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
@@ -2901,7 +3500,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
@@ -2924,12 +3523,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14" t="s">
@@ -2948,7 +3547,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
@@ -2971,7 +3570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>42</v>
       </c>
@@ -2992,7 +3591,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
         <v>43</v>
       </c>
@@ -3027,15 +3626,15 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.9296875" customWidth="1"/>
-    <col min="2" max="2" width="7.1328125" customWidth="1"/>
-    <col min="3" max="6" width="4.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="6" width="4.7109375" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>46</v>
       </c>
@@ -3047,7 +3646,7 @@
       <c r="E1" s="18"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>44</v>
       </c>
@@ -3067,7 +3666,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -3088,7 +3687,7 @@
       </c>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>2.5</v>
       </c>
@@ -3109,7 +3708,7 @@
       </c>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -3130,7 +3729,7 @@
       </c>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>3.5</v>
       </c>
@@ -3151,7 +3750,7 @@
       </c>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -3172,7 +3771,7 @@
       </c>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
@@ -3180,75 +3779,75 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
     </row>
@@ -3266,22 +3865,22 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -3289,27 +3888,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="e">
         <f ca="1">_xll.PsiOptParam(2,4)</f>
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
+        <v>#NAME?</v>
+      </c>
+      <c r="D3" s="1" t="e">
         <f ca="1">_xll.PsiOptParam(-3.5,-1.5)</f>
-        <v>-3.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -3330,7 +3929,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
@@ -3351,7 +3950,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -3361,9 +3960,9 @@
       <c r="D9" s="4">
         <v>1000</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="3" t="e">
         <f ca="1">SUMPRODUCT(C3:D3,C9:D9)</f>
-        <v>500</v>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -3383,38 +3982,38 @@
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="2" max="2" width="4.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.86328125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14" t="s">
@@ -3433,7 +4032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
@@ -3456,7 +4055,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
@@ -3479,7 +4078,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
@@ -3502,12 +4101,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14" t="s">
@@ -3526,7 +4125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
@@ -3549,7 +4148,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>42</v>
       </c>
@@ -3570,7 +4169,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
         <v>43</v>
       </c>
@@ -3605,22 +4204,22 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -3628,7 +4227,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -3639,14 +4238,14 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -3667,7 +4266,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
@@ -3688,7 +4287,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -3703,12 +4302,12 @@
         <v>3502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>48</v>
       </c>
@@ -3732,481 +4331,481 @@
       <selection activeCell="E23" sqref="E23:E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.65" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="5.9296875" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.53125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" style="31" customWidth="1"/>
-    <col min="5" max="5" width="7.796875" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.46484375" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.86328125" style="31" customWidth="1"/>
-    <col min="9" max="16384" width="9.06640625" style="31"/>
+    <col min="1" max="1" width="2.140625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="6" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="30" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="33" t="s">
+    <row r="8" spans="1:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="34" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-    </row>
-    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="36" t="s">
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36">
+      <c r="C10" s="35"/>
+      <c r="D10" s="35">
         <v>48</v>
       </c>
-      <c r="E10" s="36">
-        <v>0</v>
-      </c>
-      <c r="F10" s="36">
+      <c r="E10" s="35">
+        <v>0</v>
+      </c>
+      <c r="F10" s="35">
         <v>170</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="35">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="36" t="s">
+    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36">
+      <c r="C11" s="35"/>
+      <c r="D11" s="35">
         <v>31</v>
       </c>
-      <c r="E11" s="36">
-        <v>0</v>
-      </c>
-      <c r="F11" s="36">
+      <c r="E11" s="35">
+        <v>0</v>
+      </c>
+      <c r="F11" s="35">
         <v>160</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="35">
         <v>10</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="35">
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="36" t="s">
+    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36">
+      <c r="C12" s="35"/>
+      <c r="D12" s="35">
         <v>39</v>
       </c>
-      <c r="E12" s="36">
-        <v>0</v>
-      </c>
-      <c r="F12" s="36">
+      <c r="E12" s="35">
+        <v>0</v>
+      </c>
+      <c r="F12" s="35">
         <v>175</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="35">
         <v>5</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="35">
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="36" t="s">
+    <row r="13" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36">
+      <c r="C13" s="35"/>
+      <c r="D13" s="35">
         <v>43</v>
       </c>
-      <c r="E13" s="36">
-        <v>0</v>
-      </c>
-      <c r="F13" s="36">
+      <c r="E13" s="35">
+        <v>0</v>
+      </c>
+      <c r="F13" s="35">
         <v>180</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="35">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="37" t="s">
+    <row r="14" spans="1:8" ht="12.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37">
+      <c r="C14" s="36"/>
+      <c r="D14" s="36">
         <v>15</v>
       </c>
-      <c r="E14" s="37">
-        <v>0</v>
-      </c>
-      <c r="F14" s="37">
+      <c r="E14" s="36">
+        <v>0</v>
+      </c>
+      <c r="F14" s="36">
         <v>195</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G14" s="36">
         <v>1E+30</v>
       </c>
-      <c r="H14" s="37">
+      <c r="H14" s="36">
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-    </row>
-    <row r="17" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="31" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="17" spans="1:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="33" t="s">
+    <row r="19" spans="1:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="34" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-    </row>
-    <row r="21" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="36" t="s">
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+    </row>
+    <row r="21" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36">
+      <c r="C21" s="35"/>
+      <c r="D21" s="35">
         <v>48</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="35">
         <v>10</v>
       </c>
-      <c r="F21" s="36">
+      <c r="F21" s="35">
         <v>48</v>
       </c>
-      <c r="G21" s="36">
+      <c r="G21" s="35">
         <v>6</v>
       </c>
-      <c r="H21" s="36">
+      <c r="H21" s="35">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="36" t="s">
+    <row r="22" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36">
+      <c r="C22" s="35"/>
+      <c r="D22" s="35">
         <v>79</v>
       </c>
-      <c r="E22" s="36">
+      <c r="E22" s="35">
         <v>160</v>
       </c>
-      <c r="F22" s="36">
+      <c r="F22" s="35">
         <v>79</v>
       </c>
-      <c r="G22" s="36">
+      <c r="G22" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H22" s="36">
+      <c r="H22" s="35">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="36" t="s">
+    <row r="23" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35">
         <v>79</v>
       </c>
-      <c r="E23" s="36">
-        <v>0</v>
-      </c>
-      <c r="F23" s="36">
+      <c r="E23" s="35">
+        <v>0</v>
+      </c>
+      <c r="F23" s="35">
         <v>65</v>
       </c>
-      <c r="G23" s="36">
+      <c r="G23" s="35">
         <v>14</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H23" s="35">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="36" t="s">
+    <row r="24" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36">
+      <c r="C24" s="35"/>
+      <c r="D24" s="35">
         <v>118</v>
       </c>
-      <c r="E24" s="36">
-        <v>0</v>
-      </c>
-      <c r="F24" s="36">
+      <c r="E24" s="35">
+        <v>0</v>
+      </c>
+      <c r="F24" s="35">
         <v>87</v>
       </c>
-      <c r="G24" s="36">
+      <c r="G24" s="35">
         <v>31</v>
       </c>
-      <c r="H24" s="36">
+      <c r="H24" s="35">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="25" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="36" t="s">
+    <row r="25" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36">
+      <c r="C25" s="35"/>
+      <c r="D25" s="35">
         <v>70</v>
       </c>
-      <c r="E25" s="36">
-        <v>0</v>
-      </c>
-      <c r="F25" s="36">
+      <c r="E25" s="35">
+        <v>0</v>
+      </c>
+      <c r="F25" s="35">
         <v>64</v>
       </c>
-      <c r="G25" s="36">
+      <c r="G25" s="35">
         <v>6</v>
       </c>
-      <c r="H25" s="36">
+      <c r="H25" s="35">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="26" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="36" t="s">
+    <row r="26" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36">
+      <c r="C26" s="35"/>
+      <c r="D26" s="35">
         <v>82</v>
       </c>
-      <c r="E26" s="36">
-        <v>0</v>
-      </c>
-      <c r="F26" s="36">
+      <c r="E26" s="35">
+        <v>0</v>
+      </c>
+      <c r="F26" s="35">
         <v>73</v>
       </c>
-      <c r="G26" s="36">
+      <c r="G26" s="35">
         <v>9</v>
       </c>
-      <c r="H26" s="36">
+      <c r="H26" s="35">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="27" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="36" t="s">
+    <row r="27" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36">
+      <c r="C27" s="35"/>
+      <c r="D27" s="35">
         <v>82</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="35">
         <v>175</v>
       </c>
-      <c r="F27" s="36">
+      <c r="F27" s="35">
         <v>82</v>
       </c>
-      <c r="G27" s="36">
+      <c r="G27" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H27" s="36">
+      <c r="H27" s="35">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="36" t="s">
+    <row r="28" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36">
+      <c r="C28" s="35"/>
+      <c r="D28" s="35">
         <v>43</v>
       </c>
-      <c r="E28" s="36">
+      <c r="E28" s="35">
         <v>5</v>
       </c>
-      <c r="F28" s="36">
+      <c r="F28" s="35">
         <v>43</v>
       </c>
-      <c r="G28" s="36">
+      <c r="G28" s="35">
         <v>6</v>
       </c>
-      <c r="H28" s="36">
+      <c r="H28" s="35">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="36" t="s">
+    <row r="29" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35">
         <v>58</v>
       </c>
-      <c r="E29" s="36">
-        <v>0</v>
-      </c>
-      <c r="F29" s="36">
+      <c r="E29" s="35">
+        <v>0</v>
+      </c>
+      <c r="F29" s="35">
         <v>52</v>
       </c>
-      <c r="G29" s="36">
+      <c r="G29" s="35">
         <v>6</v>
       </c>
-      <c r="H29" s="36">
+      <c r="H29" s="35">
         <v>1E+30</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="12" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="37" t="s">
+    <row r="30" spans="1:8" ht="12.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36">
         <v>15</v>
       </c>
-      <c r="E30" s="37">
+      <c r="E30" s="36">
         <v>195</v>
       </c>
-      <c r="F30" s="37">
+      <c r="F30" s="36">
         <v>15</v>
       </c>
-      <c r="G30" s="37">
+      <c r="G30" s="36">
         <v>1E+30</v>
       </c>
-      <c r="H30" s="37">
+      <c r="H30" s="36">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4222,22 +4821,22 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="2.265625" customWidth="1"/>
-    <col min="3" max="3" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="3.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A3" s="39" t="s">
+    <row r="3" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>170</v>
       </c>
@@ -4254,7 +4853,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>1</v>
       </c>
@@ -4271,7 +4870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1</v>
       </c>
@@ -4283,7 +4882,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f>SUMPRODUCT(D7:H7,AgentsPerShift)</f>
+        <f t="shared" ref="I7:I16" si="0">SUMPRODUCT(D7:H7,AgentsPerShift)</f>
         <v>48</v>
       </c>
       <c r="J7" t="s">
@@ -4293,7 +4892,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>2</v>
       </c>
@@ -4307,7 +4906,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8">
-        <f>SUMPRODUCT(D8:H8,AgentsPerShift)</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="J8" t="s">
@@ -4317,7 +4916,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>3</v>
       </c>
@@ -4331,7 +4930,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9">
-        <f>SUMPRODUCT(D9:H9,AgentsPerShift)</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="J9" t="s">
@@ -4341,7 +4940,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>4</v>
       </c>
@@ -4357,7 +4956,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10">
-        <f>SUMPRODUCT(D10:H10,AgentsPerShift)</f>
+        <f t="shared" si="0"/>
         <v>118</v>
       </c>
       <c r="J10" t="s">
@@ -4367,7 +4966,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>5</v>
       </c>
@@ -4381,7 +4980,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11">
-        <f>SUMPRODUCT(D11:H11,AgentsPerShift)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="J11" t="s">
@@ -4391,7 +4990,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>6</v>
       </c>
@@ -4405,7 +5004,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12">
-        <f>SUMPRODUCT(D12:H12,AgentsPerShift)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="J12" t="s">
@@ -4415,7 +5014,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>7</v>
       </c>
@@ -4429,7 +5028,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13">
-        <f>SUMPRODUCT(D13:H13,AgentsPerShift)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="J13" t="s">
@@ -4439,7 +5038,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>8</v>
       </c>
@@ -4451,7 +5050,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14">
-        <f>SUMPRODUCT(D14:H14,AgentsPerShift)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="J14" t="s">
@@ -4461,7 +5060,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>9</v>
       </c>
@@ -4475,7 +5074,7 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <f>SUMPRODUCT(D15:H15,AgentsPerShift)</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="J15" t="s">
@@ -4485,7 +5084,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>10</v>
       </c>
@@ -4497,7 +5096,7 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <f>SUMPRODUCT(D16:H16,AgentsPerShift)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="J16" t="s">
@@ -4507,20 +5106,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.45">
-      <c r="D18" s="29">
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="28">
         <v>48</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="28">
         <v>31</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="28">
         <v>39</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="28">
         <v>43</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="28">
         <v>15</v>
       </c>
       <c r="K18" s="3">

</xml_diff>

<commit_message>
Added DS 775 Wk 5
</commit_message>
<xml_diff>
--- a/wk5/HW_5_Isaacson.xlsx
+++ b/wk5/HW_5_Isaacson.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myscripts\school\ds775\wk5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8565" windowHeight="7965" tabRatio="897" firstSheet="6" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8565" windowHeight="7965" tabRatio="897" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="4.7-6 Sensitivity Report" sheetId="6" r:id="rId1"/>
@@ -18,14 +18,16 @@
     <sheet name="7.3-4 Analysis Report" sheetId="13" r:id="rId4"/>
     <sheet name="7.3-4" sheetId="7" r:id="rId5"/>
     <sheet name="7.3-5 Sensitivity Report" sheetId="35" r:id="rId6"/>
-    <sheet name="7.3-5" sheetId="34" r:id="rId7"/>
-    <sheet name="7.3-7 Sensitivity Report" sheetId="39" r:id="rId8"/>
-    <sheet name="7.3-7" sheetId="38" r:id="rId9"/>
-    <sheet name="7.4-4" sheetId="40" r:id="rId10"/>
-    <sheet name="7.5-1" sheetId="42" r:id="rId11"/>
-    <sheet name="7.5-4" sheetId="43" r:id="rId12"/>
-    <sheet name="7.6-1" sheetId="44" r:id="rId13"/>
-    <sheet name="7.6-3" sheetId="45" r:id="rId14"/>
+    <sheet name="7.3-5 Analysis Report A" sheetId="46" r:id="rId7"/>
+    <sheet name="7.3-5 Analysis Report B" sheetId="48" r:id="rId8"/>
+    <sheet name="7.3-5" sheetId="34" r:id="rId9"/>
+    <sheet name="7.3-7 Sensitivity Report" sheetId="39" r:id="rId10"/>
+    <sheet name="7.3-7" sheetId="38" r:id="rId11"/>
+    <sheet name="7.4-4" sheetId="40" r:id="rId12"/>
+    <sheet name="7.5-1" sheetId="42" r:id="rId13"/>
+    <sheet name="7.5-4" sheetId="43" r:id="rId14"/>
+    <sheet name="7.6-1" sheetId="44" r:id="rId15"/>
+    <sheet name="7.6-3" sheetId="45" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="AgentsPerShift">'7.3-7'!$D$18:$H$18</definedName>
@@ -33,550 +35,550 @@
     <definedName name="AgentsPerTmePeriod">'7.3-7'!$I$7:$I$16</definedName>
     <definedName name="AgentsSelected">'7.3-7'!$I$7:$I$16</definedName>
     <definedName name="coin_cuttype" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="coin_cuttype" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="coin_cuttype" localSheetId="8" hidden="1">1</definedName>
     <definedName name="coin_dualtol" localSheetId="4" hidden="1">0.0000001</definedName>
-    <definedName name="coin_dualtol" localSheetId="6" hidden="1">0.0000001</definedName>
+    <definedName name="coin_dualtol" localSheetId="8" hidden="1">0.0000001</definedName>
     <definedName name="coin_heurs" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="coin_heurs" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="coin_heurs" localSheetId="8" hidden="1">1</definedName>
     <definedName name="coin_integerpresolve" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="coin_integerpresolve" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="coin_integerpresolve" localSheetId="8" hidden="1">1</definedName>
     <definedName name="coin_presolve1" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="coin_presolve1" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="coin_presolve1" localSheetId="8" hidden="1">1</definedName>
     <definedName name="coin_primaltol" localSheetId="4" hidden="1">0.0000001</definedName>
-    <definedName name="coin_primaltol" localSheetId="6" hidden="1">0.0000001</definedName>
-    <definedName name="constraint" localSheetId="11">#REF!</definedName>
+    <definedName name="coin_primaltol" localSheetId="8" hidden="1">0.0000001</definedName>
+    <definedName name="constraint" localSheetId="13">#REF!</definedName>
     <definedName name="constraint">#REF!</definedName>
     <definedName name="DailyCostPerAgent">'7.3-7'!$D$5:$H$5</definedName>
     <definedName name="grb_async_callbacks" localSheetId="1" hidden="1">1</definedName>
     <definedName name="grb_async_callbacks" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="grb_async_callbacks" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="grb_async_callbacks" localSheetId="8" hidden="1">1</definedName>
     <definedName name="grb_bariter" localSheetId="1" hidden="1">1E+100</definedName>
     <definedName name="grb_bariter" localSheetId="4" hidden="1">1E+100</definedName>
-    <definedName name="grb_bariter" localSheetId="6" hidden="1">1E+100</definedName>
+    <definedName name="grb_bariter" localSheetId="8" hidden="1">1E+100</definedName>
     <definedName name="grb_bartol" localSheetId="1" hidden="1">0.00000001</definedName>
     <definedName name="grb_bartol" localSheetId="4" hidden="1">0.00000001</definedName>
-    <definedName name="grb_bartol" localSheetId="6" hidden="1">0.00000001</definedName>
+    <definedName name="grb_bartol" localSheetId="8" hidden="1">0.00000001</definedName>
     <definedName name="grb_crossover" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_crossover" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_crossover" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_crossover" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_cut_passes" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_cut_passes" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_cut_passes" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_cut_passes" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_cutoff" localSheetId="1" hidden="1">1E+100</definedName>
     <definedName name="grb_cutoff" localSheetId="4" hidden="1">1E+100</definedName>
-    <definedName name="grb_cutoff" localSheetId="6" hidden="1">1E+100</definedName>
+    <definedName name="grb_cutoff" localSheetId="8" hidden="1">1E+100</definedName>
     <definedName name="grb_cuts" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_cuts" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_cuts" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_cuts" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_focus" localSheetId="1" hidden="1">0</definedName>
     <definedName name="grb_focus" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="grb_focus" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="grb_focus" localSheetId="8" hidden="1">0</definedName>
     <definedName name="grb_heur" localSheetId="1" hidden="1">0.05</definedName>
     <definedName name="grb_heur" localSheetId="4" hidden="1">0.05</definedName>
-    <definedName name="grb_heur" localSheetId="6" hidden="1">0.05</definedName>
+    <definedName name="grb_heur" localSheetId="8" hidden="1">0.05</definedName>
     <definedName name="grb_improv" localSheetId="1" hidden="1">1E+100</definedName>
     <definedName name="grb_improv" localSheetId="4" hidden="1">1E+100</definedName>
-    <definedName name="grb_improv" localSheetId="6" hidden="1">1E+100</definedName>
+    <definedName name="grb_improv" localSheetId="8" hidden="1">1E+100</definedName>
     <definedName name="grb_improv_start_gap" localSheetId="1" hidden="1">0</definedName>
     <definedName name="grb_improv_start_gap" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="grb_improv_start_gap" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="grb_improv_start_gap" localSheetId="8" hidden="1">0</definedName>
     <definedName name="grb_infeas" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="grb_infeas" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="grb_infeas" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="grb_infeas" localSheetId="8" hidden="1">0.000001</definedName>
     <definedName name="grb_inttol" localSheetId="1" hidden="1">0.00001</definedName>
     <definedName name="grb_inttol" localSheetId="4" hidden="1">0.00001</definedName>
-    <definedName name="grb_inttol" localSheetId="6" hidden="1">0.00001</definedName>
+    <definedName name="grb_inttol" localSheetId="8" hidden="1">0.00001</definedName>
     <definedName name="grb_method" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_method" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_method" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_method" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_nodefilestart" localSheetId="1" hidden="1">1E+100</definedName>
     <definedName name="grb_nodefilestart" localSheetId="4" hidden="1">1E+100</definedName>
-    <definedName name="grb_nodefilestart" localSheetId="6" hidden="1">1E+100</definedName>
+    <definedName name="grb_nodefilestart" localSheetId="8" hidden="1">1E+100</definedName>
     <definedName name="grb_optimal" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="grb_optimal" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="grb_optimal" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="grb_optimal" localSheetId="8" hidden="1">0.000001</definedName>
     <definedName name="grb_order" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_order" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_order" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_order" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_pre_passes" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_pre_passes" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_pre_passes" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_pre_passes" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_presolve" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_presolve" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_presolve" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_presolve" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_pricing" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_pricing" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_pricing" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_pricing" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_psdtol" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="grb_psdtol" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="grb_psdtol" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="grb_psdtol" localSheetId="8" hidden="1">0.000001</definedName>
     <definedName name="grb_qcptol" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="grb_qcptol" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="grb_qcptol" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="grb_qcptol" localSheetId="8" hidden="1">0.000001</definedName>
     <definedName name="grb_relmip" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="grb_relmip" localSheetId="4" hidden="1">0.0001</definedName>
-    <definedName name="grb_relmip" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="grb_relmip" localSheetId="8" hidden="1">0.0001</definedName>
     <definedName name="grb_scaleflag" localSheetId="1" hidden="1">1</definedName>
     <definedName name="grb_scaleflag" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="grb_scaleflag" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="grb_scaleflag" localSheetId="8" hidden="1">1</definedName>
     <definedName name="grb_seed" localSheetId="1" hidden="1">0</definedName>
     <definedName name="grb_seed" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="grb_seed" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="grb_seed" localSheetId="8" hidden="1">0</definedName>
     <definedName name="grb_submip" localSheetId="1" hidden="1">500</definedName>
     <definedName name="grb_submip" localSheetId="4" hidden="1">500</definedName>
-    <definedName name="grb_submip" localSheetId="6" hidden="1">500</definedName>
+    <definedName name="grb_submip" localSheetId="8" hidden="1">500</definedName>
     <definedName name="grb_symmetry" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_symmetry" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_symmetry" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_symmetry" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_threads" localSheetId="1" hidden="1">0</definedName>
     <definedName name="grb_threads" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="grb_threads" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="grb_threads" localSheetId="8" hidden="1">0</definedName>
     <definedName name="grb_var" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_var" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_var" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_var" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="grb_zeroobjnodes" localSheetId="1" hidden="1">-1</definedName>
     <definedName name="grb_zeroobjnodes" localSheetId="4" hidden="1">-1</definedName>
-    <definedName name="grb_zeroobjnodes" localSheetId="6" hidden="1">-1</definedName>
+    <definedName name="grb_zeroobjnodes" localSheetId="8" hidden="1">-1</definedName>
     <definedName name="gurobi_qp" localSheetId="1" hidden="1">0</definedName>
     <definedName name="gurobi_qp" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="gurobi_qp" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="gurobi_qp" localSheetId="8" hidden="1">0</definedName>
     <definedName name="MinimunAgentsNeeded">'7.3-7'!$K$7:$K$16</definedName>
     <definedName name="MinimunAgentsPerTimePeriod">'7.3-7'!$K$7:$K$16</definedName>
-    <definedName name="objective" localSheetId="11">#REF!</definedName>
+    <definedName name="objective" localSheetId="13">#REF!</definedName>
     <definedName name="objective">#REF!</definedName>
-    <definedName name="out" localSheetId="11">#REF!</definedName>
+    <definedName name="out" localSheetId="13">#REF!</definedName>
     <definedName name="out">#REF!</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'4.7-6'!$C$9:$F$9</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'7.3-4'!$C$9:$D$9</definedName>
-    <definedName name="solver_adj" localSheetId="6" hidden="1">'7.3-5'!$C$9:$D$9</definedName>
-    <definedName name="solver_adj" localSheetId="8" hidden="1">'7.3-7'!$D$18:$H$18</definedName>
-    <definedName name="solver_adj" localSheetId="9" hidden="1">'7.4-4'!$C$33:$E$33</definedName>
-    <definedName name="solver_adj" localSheetId="10" hidden="1">'7.5-1'!$C$9:$D$9</definedName>
-    <definedName name="solver_adj" localSheetId="11" hidden="1">'7.5-4'!$C$9:$E$9</definedName>
-    <definedName name="solver_adj" localSheetId="12" hidden="1">'7.6-1'!$C$11:$E$11</definedName>
-    <definedName name="solver_adj" localSheetId="13" hidden="1">'7.6-3'!$D$14:$G$14</definedName>
+    <definedName name="solver_adj" localSheetId="8" hidden="1">'7.3-5'!$C$9:$D$9</definedName>
+    <definedName name="solver_adj" localSheetId="10" hidden="1">'7.3-7'!$D$18:$H$18</definedName>
+    <definedName name="solver_adj" localSheetId="11" hidden="1">'7.4-4'!$C$33:$E$33</definedName>
+    <definedName name="solver_adj" localSheetId="12" hidden="1">'7.5-1'!$C$9:$D$9</definedName>
+    <definedName name="solver_adj" localSheetId="13" hidden="1">'7.5-4'!$C$9:$E$9</definedName>
+    <definedName name="solver_adj" localSheetId="14" hidden="1">'7.6-1'!$C$11:$E$11</definedName>
+    <definedName name="solver_adj" localSheetId="15" hidden="1">'7.6-3'!$D$14:$G$14</definedName>
     <definedName name="solver_adj_ob" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_adj_ob" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_adj_ob" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_adj_ob" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_cha" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_cha" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_cha" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_cha" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_chc1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_chc1" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_chc1" localSheetId="6" hidden="1">0</definedName>
-    <definedName name="solver_chc2" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_chc1" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_chc2" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_chn" localSheetId="1" hidden="1">4</definedName>
     <definedName name="solver_chn" localSheetId="4" hidden="1">4</definedName>
-    <definedName name="solver_chn" localSheetId="6" hidden="1">4</definedName>
+    <definedName name="solver_chn" localSheetId="8" hidden="1">4</definedName>
     <definedName name="solver_chp1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_chp1" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_chp1" localSheetId="6" hidden="1">0</definedName>
-    <definedName name="solver_chp2" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_chp1" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_chp2" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_cht" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_cht" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_cht" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_cht" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_cir1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_cir1" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_cir1" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_cir2" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_cir1" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_cir2" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_con" localSheetId="1" hidden="1">" "</definedName>
     <definedName name="solver_con" localSheetId="4" hidden="1">" "</definedName>
-    <definedName name="solver_con" localSheetId="6" hidden="1">" "</definedName>
+    <definedName name="solver_con" localSheetId="8" hidden="1">" "</definedName>
     <definedName name="solver_con1" localSheetId="1" hidden="1">" "</definedName>
     <definedName name="solver_con1" localSheetId="4" hidden="1">" "</definedName>
-    <definedName name="solver_con1" localSheetId="6" hidden="1">" "</definedName>
-    <definedName name="solver_con2" localSheetId="6" hidden="1">" "</definedName>
+    <definedName name="solver_con1" localSheetId="8" hidden="1">" "</definedName>
+    <definedName name="solver_con2" localSheetId="8" hidden="1">" "</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="8" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="9" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="10" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="11" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="12" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="13" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="14" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="15" hidden="1">0.0001</definedName>
     <definedName name="solver_dia" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_dia" localSheetId="4" hidden="1">5</definedName>
-    <definedName name="solver_dia" localSheetId="6" hidden="1">5</definedName>
+    <definedName name="solver_dia" localSheetId="8" hidden="1">5</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="8" hidden="1">2</definedName>
-    <definedName name="solver_drv" localSheetId="9" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="12" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="13" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="13" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="14" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">6</definedName>
-    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="8" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="11" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="12" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="13" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="14" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="13" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="14" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_eval" hidden="1">0</definedName>
     <definedName name="solver_iao" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_iao" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_iao" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_iao" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_int" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_int" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_int" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_int" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_irs" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_irs" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_irs" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_irs" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_ism" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ism" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_ism" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_ism" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="8" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="10" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="11" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="12" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="13" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="14" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="15" hidden="1">2147483647</definedName>
     <definedName name="solver_kiv" localSheetId="4" hidden="1">2E+30</definedName>
-    <definedName name="solver_kiv" localSheetId="6" hidden="1">2E+30</definedName>
+    <definedName name="solver_kiv" localSheetId="8" hidden="1">2E+30</definedName>
     <definedName name="solver_lhs_ob1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_lhs_ob1" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_lhs_ob1" localSheetId="6" hidden="1">0</definedName>
-    <definedName name="solver_lhs_ob2" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_lhs_ob1" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_lhs_ob2" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'4.7-6'!$G$6:$G$7</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">'7.3-4'!$E$6:$E$7</definedName>
-    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'7.3-5'!$E$6:$E$7</definedName>
-    <definedName name="solver_lhs1" localSheetId="8" hidden="1">'7.3-7'!$I$7:$I$16</definedName>
-    <definedName name="solver_lhs1" localSheetId="9" hidden="1">'7.4-4'!$F$29</definedName>
-    <definedName name="solver_lhs1" localSheetId="10" hidden="1">'7.5-1'!$E$5:$E$7</definedName>
-    <definedName name="solver_lhs1" localSheetId="11" hidden="1">'7.5-4'!$F$5:$F$7</definedName>
-    <definedName name="solver_lhs1" localSheetId="12" hidden="1">'7.6-1'!$F$5:$F$9</definedName>
-    <definedName name="solver_lhs1" localSheetId="13" hidden="1">'7.6-3'!$H$12</definedName>
-    <definedName name="solver_lhs2" localSheetId="6" hidden="1">'7.3-5'!$C$9</definedName>
-    <definedName name="solver_lhs2" localSheetId="9" hidden="1">'7.4-4'!$F$30</definedName>
-    <definedName name="solver_lhs2" localSheetId="13" hidden="1">'7.6-3'!$H$8:$H$11</definedName>
-    <definedName name="solver_lhs3" localSheetId="9" hidden="1">'7.4-4'!$F$31</definedName>
+    <definedName name="solver_lhs1" localSheetId="8" hidden="1">'7.3-5'!$E$6:$E$7</definedName>
+    <definedName name="solver_lhs1" localSheetId="10" hidden="1">'7.3-7'!$I$7:$I$16</definedName>
+    <definedName name="solver_lhs1" localSheetId="11" hidden="1">'7.4-4'!$F$29:$F$31</definedName>
+    <definedName name="solver_lhs1" localSheetId="12" hidden="1">'7.5-1'!$E$5:$E$7</definedName>
+    <definedName name="solver_lhs1" localSheetId="13" hidden="1">'7.5-4'!$F$5:$F$7</definedName>
+    <definedName name="solver_lhs1" localSheetId="14" hidden="1">'7.6-1'!$F$5:$F$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="15" hidden="1">'7.6-3'!$H$12</definedName>
+    <definedName name="solver_lhs2" localSheetId="8" hidden="1">'7.3-5'!$C$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="11" hidden="1">'7.4-4'!#REF!</definedName>
+    <definedName name="solver_lhs2" localSheetId="15" hidden="1">'7.6-3'!$H$8:$H$11</definedName>
+    <definedName name="solver_lhs3" localSheetId="11" hidden="1">'7.4-4'!#REF!</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_lin" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_mda" localSheetId="1" hidden="1">4</definedName>
     <definedName name="solver_mda" localSheetId="4" hidden="1">4</definedName>
-    <definedName name="solver_mda" localSheetId="6" hidden="1">4</definedName>
+    <definedName name="solver_mda" localSheetId="8" hidden="1">4</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="8" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="10" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="11" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="12" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="13" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="14" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="15" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="8" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="9" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="10" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="11" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="12" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="13" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="14" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="15" hidden="1">30</definedName>
     <definedName name="solver_mod" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_mod" localSheetId="4" hidden="1">3</definedName>
-    <definedName name="solver_mod" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_mod" localSheetId="8" hidden="1">3</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="8" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="9" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="10" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="11" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="12" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="13" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="14" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="15" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="8" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="11" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="12" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="13" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="14" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="13" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="14" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="8" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="10" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="11" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="12" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="13" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="14" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="15" hidden="1">2147483647</definedName>
     <definedName name="solver_nopt" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_nopt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nopt" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_ntr" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ntr" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_ntr" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_ntr" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_ntri" hidden="1">1000</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="6" hidden="1">2</definedName>
-    <definedName name="solver_num" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="9" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="12" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="13" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="13" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="14" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="13" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="14" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_obc" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_obc" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_obc" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_obc" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_obp" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_obp" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_obp" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_obp" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'4.7-6'!$I$9</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">'7.3-4'!$G$9</definedName>
-    <definedName name="solver_opt" localSheetId="6" hidden="1">'7.3-5'!$G$9</definedName>
-    <definedName name="solver_opt" localSheetId="8" hidden="1">'7.3-7'!$K$18</definedName>
-    <definedName name="solver_opt" localSheetId="9" hidden="1">'7.4-4'!$H$33</definedName>
-    <definedName name="solver_opt" localSheetId="10" hidden="1">'7.5-1'!$G$9</definedName>
-    <definedName name="solver_opt" localSheetId="11" hidden="1">'7.5-4'!$H$9</definedName>
-    <definedName name="solver_opt" localSheetId="12" hidden="1">'7.6-1'!$H$11</definedName>
-    <definedName name="solver_opt" localSheetId="13" hidden="1">'7.6-3'!$J$14</definedName>
+    <definedName name="solver_opt" localSheetId="8" hidden="1">'7.3-5'!$G$9</definedName>
+    <definedName name="solver_opt" localSheetId="10" hidden="1">'7.3-7'!$K$18</definedName>
+    <definedName name="solver_opt" localSheetId="11" hidden="1">'7.4-4'!$H$33</definedName>
+    <definedName name="solver_opt" localSheetId="12" hidden="1">'7.5-1'!$G$9</definedName>
+    <definedName name="solver_opt" localSheetId="13" hidden="1">'7.5-4'!$H$9</definedName>
+    <definedName name="solver_opt" localSheetId="14" hidden="1">'7.6-1'!$H$11</definedName>
+    <definedName name="solver_opt" localSheetId="15" hidden="1">'7.6-3'!$J$14</definedName>
     <definedName name="solver_opt_ob" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt_ob" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_opt_ob" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_opt_ob" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="8" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="9" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="10" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="11" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="12" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="13" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="14" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="15" hidden="1">0.000001</definedName>
     <definedName name="solver_psi" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_psi" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_psi" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_psi" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="8" hidden="1">2</definedName>
-    <definedName name="solver_rbv" localSheetId="9" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="12" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="13" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="13" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="14" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_rdp" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rdp" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_rdp" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_rdp" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_reco1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_reco1" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_reco1" localSheetId="6" hidden="1">0</definedName>
-    <definedName name="solver_reco2" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_reco1" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_reco2" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="8" hidden="1">3</definedName>
-    <definedName name="solver_rel1" localSheetId="9" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="10" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="12" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="13" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="9" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="13" hidden="1">1</definedName>
-    <definedName name="solver_rel3" localSheetId="9" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="13" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="14" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="15" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="11" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="15" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_rep" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rep" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_rep" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_rep" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'4.7-6'!$I$6:$I$7</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">'7.3-4'!$G$6:$G$7</definedName>
-    <definedName name="solver_rhs1" localSheetId="6" hidden="1">'7.3-5'!$G$6:$G$7</definedName>
-    <definedName name="solver_rhs1" localSheetId="8" hidden="1">MinimunAgentsNeeded</definedName>
-    <definedName name="solver_rhs1" localSheetId="9" hidden="1">'7.4-4'!$H$29</definedName>
-    <definedName name="solver_rhs1" localSheetId="10" hidden="1">'7.5-1'!$G$5:$G$7</definedName>
-    <definedName name="solver_rhs1" localSheetId="11" hidden="1">'7.5-4'!$H$5:$H$7</definedName>
-    <definedName name="solver_rhs1" localSheetId="12" hidden="1">'7.6-1'!$H$5:$H$9</definedName>
-    <definedName name="solver_rhs1" localSheetId="13" hidden="1">'7.6-3'!$J$12</definedName>
-    <definedName name="solver_rhs2" localSheetId="6" hidden="1">'7.3-5'!$C$11</definedName>
-    <definedName name="solver_rhs2" localSheetId="9" hidden="1">'7.4-4'!$H$30</definedName>
-    <definedName name="solver_rhs2" localSheetId="13" hidden="1">'7.6-3'!$J$8:$J$11</definedName>
-    <definedName name="solver_rhs3" localSheetId="9" hidden="1">'7.4-4'!$H$31</definedName>
+    <definedName name="solver_rhs1" localSheetId="8" hidden="1">'7.3-5'!$G$6:$G$7</definedName>
+    <definedName name="solver_rhs1" localSheetId="10" hidden="1">MinimunAgentsNeeded</definedName>
+    <definedName name="solver_rhs1" localSheetId="11" hidden="1">'7.4-4'!$H$29:$H$31</definedName>
+    <definedName name="solver_rhs1" localSheetId="12" hidden="1">'7.5-1'!$G$5:$G$7</definedName>
+    <definedName name="solver_rhs1" localSheetId="13" hidden="1">'7.5-4'!$H$5:$H$7</definedName>
+    <definedName name="solver_rhs1" localSheetId="14" hidden="1">'7.6-1'!$H$5:$H$9</definedName>
+    <definedName name="solver_rhs1" localSheetId="15" hidden="1">'7.6-3'!$J$12</definedName>
+    <definedName name="solver_rhs2" localSheetId="8" hidden="1">'7.3-5'!$C$11</definedName>
+    <definedName name="solver_rhs2" localSheetId="11" hidden="1">'7.4-4'!#REF!</definedName>
+    <definedName name="solver_rhs2" localSheetId="15" hidden="1">'7.6-3'!$J$8:$J$11</definedName>
+    <definedName name="solver_rhs3" localSheetId="11" hidden="1">'7.4-4'!#REF!</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="8" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_rlx" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="11" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="12" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="13" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="14" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="8" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="9" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="10" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="11" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="12" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="13" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="14" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="15" hidden="1">0</definedName>
     <definedName name="solver_rsmp" hidden="1">2</definedName>
     <definedName name="solver_rtr" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rtr" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_rtr" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_rtr" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_rxc1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rxc1" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rxc1" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_rxc2" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rxc1" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_rxc2" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_rxv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rxv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rxv" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rxv" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="8" hidden="1">2</definedName>
-    <definedName name="solver_scl" localSheetId="9" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="12" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="13" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="13" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="14" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_seed" hidden="1">0</definedName>
     <definedName name="solver_sel" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sel" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_sel" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_sel" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="8" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="11" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="12" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="13" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="14" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_slv" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_slv" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_slv" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_slv" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_slvu" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_slvu" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_slvu" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_slvu" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_spid" localSheetId="1" hidden="1">" "</definedName>
     <definedName name="solver_spid" localSheetId="4" hidden="1">" "</definedName>
-    <definedName name="solver_spid" localSheetId="6" hidden="1">" "</definedName>
+    <definedName name="solver_spid" localSheetId="8" hidden="1">" "</definedName>
     <definedName name="solver_srvr" localSheetId="1" hidden="1">" "</definedName>
     <definedName name="solver_srvr" localSheetId="4" hidden="1">" "</definedName>
-    <definedName name="solver_srvr" localSheetId="6" hidden="1">" "</definedName>
+    <definedName name="solver_srvr" localSheetId="8" hidden="1">" "</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="8" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="9" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="10" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="11" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="12" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="13" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="14" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="15" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="8" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="10" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="11" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="12" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="13" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="14" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="15" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="8" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="9" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="10" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="11" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="12" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="13" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="14" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="15" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="8" hidden="1">2</definedName>
-    <definedName name="solver_typ" localSheetId="9" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="10" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="11" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="13" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="14" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_umod" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_umod" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_umod" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_umod" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_urs" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_urs" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_urs" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_urs" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_userid" localSheetId="1" hidden="1">319624</definedName>
     <definedName name="solver_userid" localSheetId="4" hidden="1">319624</definedName>
-    <definedName name="solver_userid" localSheetId="6" hidden="1">319624</definedName>
     <definedName name="solver_userid" localSheetId="8" hidden="1">319624</definedName>
-    <definedName name="solver_userid" localSheetId="9" hidden="1">319624</definedName>
+    <definedName name="solver_userid" localSheetId="10" hidden="1">319624</definedName>
+    <definedName name="solver_userid" localSheetId="11" hidden="1">319624</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="8" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="9" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="10" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="11" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="12" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="13" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="14" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="15" hidden="1">0</definedName>
     <definedName name="solver_var" localSheetId="1" hidden="1">" "</definedName>
     <definedName name="solver_var" localSheetId="4" hidden="1">" "</definedName>
-    <definedName name="solver_var" localSheetId="6" hidden="1">" "</definedName>
+    <definedName name="solver_var" localSheetId="8" hidden="1">" "</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">16</definedName>
-    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="8" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="9" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="8" hidden="1">16</definedName>
     <definedName name="solver_ver" localSheetId="10" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="11" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="12" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="13" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="14" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="15" hidden="1">3</definedName>
     <definedName name="solver_vir" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_vir" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_vir" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_vir" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_vol" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_vol" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_vol" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_vol" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_vst" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_vst" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_vst" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_vst" localSheetId="8" hidden="1">0</definedName>
     <definedName name="TotalCost">'7.3-7'!$K$18</definedName>
-    <definedName name="var" localSheetId="11">#REF!</definedName>
+    <definedName name="var" localSheetId="13">#REF!</definedName>
     <definedName name="var">#REF!</definedName>
-    <definedName name="variable" localSheetId="11">#REF!</definedName>
+    <definedName name="variable" localSheetId="13">#REF!</definedName>
     <definedName name="variable">#REF!</definedName>
   </definedNames>
   <calcPr calcId="171027" calcOnSave="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId15"/>
+    <pivotCache cacheId="0" r:id="rId17"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -587,7 +589,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="96">
   <si>
     <t>&gt;=</t>
   </si>
@@ -872,6 +874,9 @@
   </si>
   <si>
     <t>0.5*x1 + 0.50x21 + 0.005x22 + 0x23</t>
+  </si>
+  <si>
+    <t>$G$9</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1007,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1250,13 +1255,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -1385,10 +1401,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
@@ -1956,39 +1977,39 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.1328125" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.265625" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.86328125" customWidth="1"/>
+    <col min="8" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
@@ -2007,7 +2028,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
@@ -2030,7 +2051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" s="13" t="s">
         <v>37</v>
       </c>
@@ -2041,7 +2062,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
@@ -2064,7 +2085,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
         <v>29</v>
       </c>
@@ -2087,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
@@ -2110,7 +2131,7 @@
         <v>1.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="14.65" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="9" t="s">
         <v>33</v>
       </c>
@@ -2133,7 +2154,7 @@
         <v>1.3333333333333335</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -2142,12 +2163,12 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
@@ -2166,7 +2187,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
@@ -2189,7 +2210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
@@ -2210,7 +2231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B20" s="9" t="s">
         <v>36</v>
       </c>
@@ -2238,29 +2259,846 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="N10" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23:E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.65" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1328125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="6" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.59765625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="5.265625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="7.86328125" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.86328125" style="30" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35">
+        <v>48</v>
+      </c>
+      <c r="E10" s="35">
+        <v>0</v>
+      </c>
+      <c r="F10" s="35">
+        <v>170</v>
+      </c>
+      <c r="G10" s="35">
+        <v>1E+30</v>
+      </c>
+      <c r="H10" s="35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35">
+        <v>31</v>
+      </c>
+      <c r="E11" s="35">
+        <v>0</v>
+      </c>
+      <c r="F11" s="35">
+        <v>160</v>
+      </c>
+      <c r="G11" s="35">
+        <v>10</v>
+      </c>
+      <c r="H11" s="35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35">
+        <v>39</v>
+      </c>
+      <c r="E12" s="35">
+        <v>0</v>
+      </c>
+      <c r="F12" s="35">
+        <v>175</v>
+      </c>
+      <c r="G12" s="35">
+        <v>5</v>
+      </c>
+      <c r="H12" s="35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35">
+        <v>43</v>
+      </c>
+      <c r="E13" s="35">
+        <v>0</v>
+      </c>
+      <c r="F13" s="35">
+        <v>180</v>
+      </c>
+      <c r="G13" s="35">
+        <v>1E+30</v>
+      </c>
+      <c r="H13" s="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="12" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36">
+        <v>15</v>
+      </c>
+      <c r="E14" s="36">
+        <v>0</v>
+      </c>
+      <c r="F14" s="36">
+        <v>195</v>
+      </c>
+      <c r="G14" s="36">
+        <v>1E+30</v>
+      </c>
+      <c r="H14" s="36">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="17" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+    </row>
+    <row r="21" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35">
+        <v>48</v>
+      </c>
+      <c r="E21" s="35">
+        <v>10</v>
+      </c>
+      <c r="F21" s="35">
+        <v>48</v>
+      </c>
+      <c r="G21" s="35">
+        <v>6</v>
+      </c>
+      <c r="H21" s="35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35">
+        <v>79</v>
+      </c>
+      <c r="E22" s="35">
+        <v>160</v>
+      </c>
+      <c r="F22" s="35">
+        <v>79</v>
+      </c>
+      <c r="G22" s="35">
+        <v>1E+30</v>
+      </c>
+      <c r="H22" s="35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35">
+        <v>79</v>
+      </c>
+      <c r="E23" s="35">
+        <v>0</v>
+      </c>
+      <c r="F23" s="35">
+        <v>65</v>
+      </c>
+      <c r="G23" s="35">
+        <v>14</v>
+      </c>
+      <c r="H23" s="35">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35">
+        <v>118</v>
+      </c>
+      <c r="E24" s="35">
+        <v>0</v>
+      </c>
+      <c r="F24" s="35">
+        <v>87</v>
+      </c>
+      <c r="G24" s="35">
+        <v>31</v>
+      </c>
+      <c r="H24" s="35">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35">
+        <v>70</v>
+      </c>
+      <c r="E25" s="35">
+        <v>0</v>
+      </c>
+      <c r="F25" s="35">
+        <v>64</v>
+      </c>
+      <c r="G25" s="35">
+        <v>6</v>
+      </c>
+      <c r="H25" s="35">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35">
+        <v>82</v>
+      </c>
+      <c r="E26" s="35">
+        <v>0</v>
+      </c>
+      <c r="F26" s="35">
+        <v>73</v>
+      </c>
+      <c r="G26" s="35">
+        <v>9</v>
+      </c>
+      <c r="H26" s="35">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35">
+        <v>82</v>
+      </c>
+      <c r="E27" s="35">
+        <v>175</v>
+      </c>
+      <c r="F27" s="35">
+        <v>82</v>
+      </c>
+      <c r="G27" s="35">
+        <v>1E+30</v>
+      </c>
+      <c r="H27" s="35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35">
+        <v>43</v>
+      </c>
+      <c r="E28" s="35">
+        <v>5</v>
+      </c>
+      <c r="F28" s="35">
+        <v>43</v>
+      </c>
+      <c r="G28" s="35">
+        <v>6</v>
+      </c>
+      <c r="H28" s="35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35">
+        <v>58</v>
+      </c>
+      <c r="E29" s="35">
+        <v>0</v>
+      </c>
+      <c r="F29" s="35">
+        <v>52</v>
+      </c>
+      <c r="G29" s="35">
+        <v>6</v>
+      </c>
+      <c r="H29" s="35">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="12" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36">
+        <v>15</v>
+      </c>
+      <c r="E30" s="36">
+        <v>195</v>
+      </c>
+      <c r="F30" s="36">
+        <v>15</v>
+      </c>
+      <c r="G30" s="36">
+        <v>1E+30</v>
+      </c>
+      <c r="H30" s="36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="2.265625" customWidth="1"/>
+    <col min="3" max="3" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A3" s="38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="D5" s="1">
+        <v>170</v>
+      </c>
+      <c r="E5" s="1">
+        <v>160</v>
+      </c>
+      <c r="F5" s="1">
+        <v>175</v>
+      </c>
+      <c r="G5" s="1">
+        <v>180</v>
+      </c>
+      <c r="H5" s="1">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7">
+        <f t="shared" ref="I7:I16" si="0">SUMPRODUCT(D7:H7,AgentsPerShift)</f>
+        <v>48</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="J8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="J11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="J14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.45">
+      <c r="D18" s="28">
+        <v>48</v>
+      </c>
+      <c r="E18" s="28">
+        <v>31</v>
+      </c>
+      <c r="F18" s="28">
+        <v>39</v>
+      </c>
+      <c r="G18" s="28">
+        <v>43</v>
+      </c>
+      <c r="H18" s="28">
+        <v>15</v>
+      </c>
+      <c r="K18" s="3">
+        <f>SUMPRODUCT(DailyCostPerAgent,AgentsPerShift)</f>
+        <v>30610</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.06640625" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.59765625" customWidth="1"/>
+    <col min="15" max="15" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.9296875" customWidth="1"/>
+    <col min="17" max="17" width="4.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="38" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C3" s="39" t="s">
         <v>72</v>
       </c>
@@ -2274,7 +3112,7 @@
       <c r="G3" s="40"/>
       <c r="H3" s="41"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C4" s="42"/>
       <c r="D4" s="43"/>
       <c r="E4" s="43"/>
@@ -2282,7 +3120,7 @@
       <c r="G4" s="43"/>
       <c r="H4" s="44"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C5" s="42" t="s">
         <v>74</v>
       </c>
@@ -2300,7 +3138,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C6" s="42" t="s">
         <v>78</v>
       </c>
@@ -2318,7 +3156,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C7" s="42" t="s">
         <v>81</v>
       </c>
@@ -2336,7 +3174,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C8" s="42"/>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
@@ -2344,7 +3182,7 @@
       <c r="G8" s="43"/>
       <c r="H8" s="44"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C9" s="45"/>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
@@ -2352,7 +3190,7 @@
       <c r="G9" s="46"/>
       <c r="H9" s="47"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C11" s="48">
         <v>5</v>
       </c>
@@ -2366,7 +3204,7 @@
       <c r="G11" s="49"/>
       <c r="H11" s="50"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C12" s="51"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
@@ -2374,7 +3212,7 @@
       <c r="G12" s="52"/>
       <c r="H12" s="53"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C13" s="51" t="s">
         <v>74</v>
       </c>
@@ -2392,7 +3230,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C14" s="51">
         <v>3</v>
       </c>
@@ -2410,7 +3248,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C15" s="51">
         <v>2</v>
       </c>
@@ -2428,7 +3266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C16" s="42"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
@@ -2436,7 +3274,7 @@
       <c r="G16" s="43"/>
       <c r="H16" s="44"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C17" s="45"/>
       <c r="D17" s="46"/>
       <c r="E17" s="46"/>
@@ -2444,7 +3282,7 @@
       <c r="G17" s="46"/>
       <c r="H17" s="47"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C19" s="54">
         <v>5</v>
       </c>
@@ -2458,7 +3296,7 @@
       <c r="G19" s="55"/>
       <c r="H19" s="56"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C20" s="57"/>
       <c r="D20" s="58"/>
       <c r="E20" s="58"/>
@@ -2466,7 +3304,7 @@
       <c r="G20" s="58"/>
       <c r="H20" s="59"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C21" s="63">
         <v>4</v>
       </c>
@@ -2478,7 +3316,7 @@
       </c>
       <c r="F21" s="58">
         <f>SUMPRODUCT(C21:E21,$C$25:$E$25)</f>
-        <v>30</v>
+        <v>28.571428571428569</v>
       </c>
       <c r="G21" s="58" t="s">
         <v>39</v>
@@ -2487,7 +3325,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C22" s="57">
         <v>3</v>
       </c>
@@ -2499,16 +3337,16 @@
       </c>
       <c r="F22" s="58">
         <f t="shared" ref="F22:F23" si="0">SUMPRODUCT(C22:E22,$C$25:$E$25)</f>
-        <v>21.25</v>
+        <v>19.999999999999996</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="H22" s="65">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C23" s="57">
         <v>2</v>
       </c>
@@ -2529,7 +3367,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C24" s="57"/>
       <c r="D24" s="58"/>
       <c r="E24" s="58"/>
@@ -2537,24 +3375,24 @@
       <c r="G24" s="58"/>
       <c r="H24" s="59"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C25" s="60">
-        <v>6.25</v>
+        <v>5.7142857142857135</v>
       </c>
       <c r="D25" s="61">
         <v>0</v>
       </c>
       <c r="E25" s="61">
-        <v>2.5</v>
+        <v>2.8571428571428577</v>
       </c>
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
       <c r="H25" s="67">
         <f>SUMPRODUCT(C19:E19,C25:E25)</f>
-        <v>41.25</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C27" s="54">
         <v>5</v>
       </c>
@@ -2568,7 +3406,7 @@
       <c r="G27" s="55"/>
       <c r="H27" s="56"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C28" s="57"/>
       <c r="D28" s="58"/>
       <c r="E28" s="58"/>
@@ -2576,7 +3414,7 @@
       <c r="G28" s="58"/>
       <c r="H28" s="59"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C29" s="63">
         <v>4.4000000000000004</v>
       </c>
@@ -2597,28 +3435,28 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C30" s="57">
         <v>3</v>
       </c>
       <c r="D30" s="62">
-        <v>-1.4</v>
+        <v>-0.6</v>
       </c>
       <c r="E30" s="58">
         <v>1</v>
       </c>
       <c r="F30" s="58">
         <f t="shared" ref="F30:F31" si="1">SUMPRODUCT(C30:E30,$C$33:$E$33)</f>
-        <v>19</v>
+        <v>17.32456140350877</v>
       </c>
       <c r="G30" s="58" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="H30" s="65">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C31" s="57">
         <v>2</v>
       </c>
@@ -2630,7 +3468,7 @@
       </c>
       <c r="F31" s="58">
         <f t="shared" si="1"/>
-        <v>9.8591549295774517</v>
+        <v>20</v>
       </c>
       <c r="G31" s="58" t="s">
         <v>39</v>
@@ -2639,7 +3477,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C32" s="57"/>
       <c r="D32" s="58"/>
       <c r="E32" s="58"/>
@@ -2647,25 +3485,25 @@
       <c r="G32" s="58"/>
       <c r="H32" s="59"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C33" s="60">
-        <v>6.7605633802816918</v>
+        <v>4.780701754385964</v>
       </c>
       <c r="D33" s="61">
-        <v>0.91549295774648287</v>
+        <v>0</v>
       </c>
       <c r="E33" s="61">
-        <v>0</v>
+        <v>2.982456140350878</v>
       </c>
       <c r="F33" s="61"/>
       <c r="G33" s="61"/>
       <c r="H33" s="67">
         <f>SUMPRODUCT(C27:E27,C33:E33)</f>
-        <v>25.563380281690115</v>
+        <v>32.850877192982452</v>
       </c>
       <c r="I33" s="66">
         <f>(H33-H25)/H25</f>
-        <v>-0.38028169014084567</v>
+        <v>-0.17872807017543871</v>
       </c>
     </row>
   </sheetData>
@@ -2673,7 +3511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -2681,24 +3519,24 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" customWidth="1"/>
-    <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.86328125" customWidth="1"/>
+    <col min="3" max="3" width="4.86328125" customWidth="1"/>
+    <col min="4" max="4" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.265625" customWidth="1"/>
+    <col min="6" max="6" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="38" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C3" s="1">
         <v>3</v>
       </c>
@@ -2706,7 +3544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -2724,7 +3562,7 @@
         <v>3.77</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C6" s="1">
         <v>0</v>
       </c>
@@ -2742,7 +3580,7 @@
         <v>11.42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -2760,7 +3598,7 @@
         <v>16.84</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C9" s="28">
         <v>1.8066666666666666</v>
       </c>
@@ -2777,7 +3615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -2785,24 +3623,24 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" customWidth="1"/>
-    <col min="4" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" customWidth="1"/>
-    <col min="7" max="7" width="2.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="3.86328125" customWidth="1"/>
+    <col min="3" max="3" width="4.86328125" customWidth="1"/>
+    <col min="4" max="5" width="4.73046875" customWidth="1"/>
+    <col min="6" max="6" width="5.265625" customWidth="1"/>
+    <col min="7" max="7" width="2.59765625" customWidth="1"/>
+    <col min="8" max="8" width="8.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="38" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C3" s="1">
         <v>20</v>
       </c>
@@ -2813,7 +3651,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C5" s="1">
         <v>3</v>
       </c>
@@ -2834,7 +3672,7 @@
         <v>84.12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -2855,7 +3693,7 @@
         <v>140.16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C7" s="1">
         <v>1</v>
       </c>
@@ -2876,7 +3714,7 @@
         <v>168.48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C9" s="28">
         <v>7.0200000000000031</v>
       </c>
@@ -2896,7 +3734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -2904,13 +3742,13 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="1.5703125" customWidth="1"/>
-    <col min="3" max="8" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="1.59765625" customWidth="1"/>
+    <col min="3" max="8" width="4.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="38" t="s">
         <v>89</v>
       </c>
@@ -2918,12 +3756,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C3" s="1">
         <v>3</v>
       </c>
@@ -2934,7 +3772,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -2955,7 +3793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C6" s="1">
         <v>0</v>
       </c>
@@ -2976,7 +3814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C7" s="1">
         <v>0</v>
       </c>
@@ -2997,7 +3835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -3018,7 +3856,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C9" s="1">
         <v>3</v>
       </c>
@@ -3039,7 +3877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C11" s="28">
         <v>2</v>
       </c>
@@ -3049,7 +3887,7 @@
       <c r="E11" s="28">
         <v>2</v>
       </c>
-      <c r="H11" s="69">
+      <c r="H11" s="68">
         <f>SUMPRODUCT(C3:E3,C11:E11)</f>
         <v>22</v>
       </c>
@@ -3060,37 +3898,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="3" width="1.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" customWidth="1"/>
+    <col min="2" max="3" width="1.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="38" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D6" s="1">
         <v>0.5</v>
       </c>
@@ -3104,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D8" s="1">
         <v>1</v>
       </c>
@@ -3128,7 +3966,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D9" s="1">
         <v>1</v>
       </c>
@@ -3150,7 +3988,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D10" s="1">
         <v>1</v>
       </c>
@@ -3174,7 +4012,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D11" s="1">
         <v>1</v>
       </c>
@@ -3198,7 +4036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D12" s="1">
         <v>1</v>
       </c>
@@ -3222,7 +4060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D14" s="28">
         <v>5</v>
       </c>
@@ -3257,22 +4095,22 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -3286,7 +4124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -3303,16 +4141,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>1</v>
       </c>
@@ -3339,7 +4177,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>2</v>
       </c>
@@ -3366,7 +4204,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -3404,38 +4242,38 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.1328125" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.265625" customWidth="1"/>
+    <col min="5" max="5" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14" t="s">
@@ -3454,7 +4292,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
@@ -3477,7 +4315,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
@@ -3500,7 +4338,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
@@ -3523,12 +4361,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14" t="s">
@@ -3547,7 +4385,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
@@ -3570,7 +4408,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="s">
         <v>42</v>
       </c>
@@ -3591,7 +4429,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B16" s="9" t="s">
         <v>43</v>
       </c>
@@ -3626,15 +4464,15 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="6" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.1328125" customWidth="1"/>
+    <col min="3" max="6" width="4.73046875" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>46</v>
       </c>
@@ -3646,7 +4484,7 @@
       <c r="E1" s="18"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="17" t="s">
         <v>44</v>
       </c>
@@ -3666,7 +4504,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -3687,7 +4525,7 @@
       </c>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="22">
         <v>2.5</v>
       </c>
@@ -3708,7 +4546,7 @@
       </c>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -3729,7 +4567,7 @@
       </c>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="22">
         <v>3.5</v>
       </c>
@@ -3750,7 +4588,7 @@
       </c>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -3771,7 +4609,7 @@
       </c>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
@@ -3779,75 +4617,75 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
     </row>
@@ -3865,22 +4703,22 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -3888,27 +4726,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="e">
+      <c r="C3" s="1">
         <f ca="1">_xll.PsiOptParam(2,4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D3" s="1" t="e">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
         <f ca="1">_xll.PsiOptParam(-3.5,-1.5)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>1</v>
       </c>
@@ -3929,7 +4767,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>2</v>
       </c>
@@ -3950,7 +4788,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -3960,9 +4798,9 @@
       <c r="D9" s="4">
         <v>1000</v>
       </c>
-      <c r="G9" s="3" t="e">
+      <c r="G9" s="3">
         <f ca="1">SUMPRODUCT(C3:D3,C9:D9)</f>
-        <v>#NAME?</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -3982,38 +4820,38 @@
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.1328125" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.265625" customWidth="1"/>
+    <col min="5" max="5" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14" t="s">
@@ -4032,7 +4870,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
@@ -4055,7 +4893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
@@ -4078,7 +4916,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
@@ -4101,12 +4939,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14" t="s">
@@ -4125,7 +4963,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
@@ -4148,7 +4986,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="s">
         <v>42</v>
       </c>
@@ -4169,7 +5007,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B16" s="9" t="s">
         <v>43</v>
       </c>
@@ -4197,29 +5035,403 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="4.9296875" customWidth="1"/>
+    <col min="2" max="2" width="4.73046875" customWidth="1"/>
+    <col min="3" max="4" width="4.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="69">
+        <v>3000</v>
+      </c>
+      <c r="B2" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C2" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="69">
+        <v>3100</v>
+      </c>
+      <c r="B3" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="69">
+        <v>3200</v>
+      </c>
+      <c r="B4" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="69">
+        <v>3300</v>
+      </c>
+      <c r="B5" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="69">
+        <v>3400</v>
+      </c>
+      <c r="B6" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C6" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="69">
+        <v>3500</v>
+      </c>
+      <c r="B7" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C7" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="69">
+        <v>3600</v>
+      </c>
+      <c r="B8" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C8" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="69">
+        <v>3700</v>
+      </c>
+      <c r="B9" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C9" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="69">
+        <v>3800</v>
+      </c>
+      <c r="B10" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C10" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="69">
+        <v>3900</v>
+      </c>
+      <c r="B11" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C11" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="70">
+        <v>4000</v>
+      </c>
+      <c r="B12" s="70">
+        <v>2000</v>
+      </c>
+      <c r="C12" s="70">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="70">
+        <v>3500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="4.9296875" customWidth="1"/>
+    <col min="2" max="2" width="4.73046875" customWidth="1"/>
+    <col min="3" max="4" width="4.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="69">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C2" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="69">
+        <v>1100</v>
+      </c>
+      <c r="B3" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="69">
+        <v>1200</v>
+      </c>
+      <c r="B4" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="69">
+        <v>1300</v>
+      </c>
+      <c r="B5" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="69">
+        <v>1400</v>
+      </c>
+      <c r="B6" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C6" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="69">
+        <v>1500</v>
+      </c>
+      <c r="B7" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C7" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="69">
+        <v>1600</v>
+      </c>
+      <c r="B8" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C8" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="69">
+        <v>1700</v>
+      </c>
+      <c r="B9" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C9" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="69">
+        <v>1800</v>
+      </c>
+      <c r="B10" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C10" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="69">
+        <v>1900</v>
+      </c>
+      <c r="B11" s="69">
+        <v>2000</v>
+      </c>
+      <c r="C11" s="69">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="69">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="70">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="70">
+        <v>2000</v>
+      </c>
+      <c r="C12" s="70">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="70">
+        <v>3500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -4227,7 +5439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -4238,14 +5450,14 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>1</v>
       </c>
@@ -4266,7 +5478,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>2</v>
       </c>
@@ -4278,36 +5490,37 @@
       </c>
       <c r="E7">
         <f>SUMPRODUCT(C7:D7,$C$9:$D$9)</f>
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>
       </c>
       <c r="G7">
+        <f ca="1">_xll.PsiOptParam(1000,2000)</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="4">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D9" s="4">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="G9" s="3">
         <f>SUMPRODUCT(C3:D3,C9:D9)</f>
-        <v>3502</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>48</v>
       </c>
@@ -4321,813 +5534,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.140625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="6" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="30" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="30"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-    </row>
-    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35">
-        <v>48</v>
-      </c>
-      <c r="E10" s="35">
-        <v>0</v>
-      </c>
-      <c r="F10" s="35">
-        <v>170</v>
-      </c>
-      <c r="G10" s="35">
-        <v>1E+30</v>
-      </c>
-      <c r="H10" s="35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35">
-        <v>31</v>
-      </c>
-      <c r="E11" s="35">
-        <v>0</v>
-      </c>
-      <c r="F11" s="35">
-        <v>160</v>
-      </c>
-      <c r="G11" s="35">
-        <v>10</v>
-      </c>
-      <c r="H11" s="35">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35">
-        <v>39</v>
-      </c>
-      <c r="E12" s="35">
-        <v>0</v>
-      </c>
-      <c r="F12" s="35">
-        <v>175</v>
-      </c>
-      <c r="G12" s="35">
-        <v>5</v>
-      </c>
-      <c r="H12" s="35">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35">
-        <v>43</v>
-      </c>
-      <c r="E13" s="35">
-        <v>0</v>
-      </c>
-      <c r="F13" s="35">
-        <v>180</v>
-      </c>
-      <c r="G13" s="35">
-        <v>1E+30</v>
-      </c>
-      <c r="H13" s="35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="12.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36">
-        <v>15</v>
-      </c>
-      <c r="E14" s="36">
-        <v>0</v>
-      </c>
-      <c r="F14" s="36">
-        <v>195</v>
-      </c>
-      <c r="G14" s="36">
-        <v>1E+30</v>
-      </c>
-      <c r="H14" s="36">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-    </row>
-    <row r="17" spans="1:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-    </row>
-    <row r="21" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35">
-        <v>48</v>
-      </c>
-      <c r="E21" s="35">
-        <v>10</v>
-      </c>
-      <c r="F21" s="35">
-        <v>48</v>
-      </c>
-      <c r="G21" s="35">
-        <v>6</v>
-      </c>
-      <c r="H21" s="35">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35">
-        <v>79</v>
-      </c>
-      <c r="E22" s="35">
-        <v>160</v>
-      </c>
-      <c r="F22" s="35">
-        <v>79</v>
-      </c>
-      <c r="G22" s="35">
-        <v>1E+30</v>
-      </c>
-      <c r="H22" s="35">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35">
-        <v>79</v>
-      </c>
-      <c r="E23" s="35">
-        <v>0</v>
-      </c>
-      <c r="F23" s="35">
-        <v>65</v>
-      </c>
-      <c r="G23" s="35">
-        <v>14</v>
-      </c>
-      <c r="H23" s="35">
-        <v>1E+30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35">
-        <v>118</v>
-      </c>
-      <c r="E24" s="35">
-        <v>0</v>
-      </c>
-      <c r="F24" s="35">
-        <v>87</v>
-      </c>
-      <c r="G24" s="35">
-        <v>31</v>
-      </c>
-      <c r="H24" s="35">
-        <v>1E+30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35">
-        <v>70</v>
-      </c>
-      <c r="E25" s="35">
-        <v>0</v>
-      </c>
-      <c r="F25" s="35">
-        <v>64</v>
-      </c>
-      <c r="G25" s="35">
-        <v>6</v>
-      </c>
-      <c r="H25" s="35">
-        <v>1E+30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35">
-        <v>82</v>
-      </c>
-      <c r="E26" s="35">
-        <v>0</v>
-      </c>
-      <c r="F26" s="35">
-        <v>73</v>
-      </c>
-      <c r="G26" s="35">
-        <v>9</v>
-      </c>
-      <c r="H26" s="35">
-        <v>1E+30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35">
-        <v>82</v>
-      </c>
-      <c r="E27" s="35">
-        <v>175</v>
-      </c>
-      <c r="F27" s="35">
-        <v>82</v>
-      </c>
-      <c r="G27" s="35">
-        <v>1E+30</v>
-      </c>
-      <c r="H27" s="35">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35">
-        <v>43</v>
-      </c>
-      <c r="E28" s="35">
-        <v>5</v>
-      </c>
-      <c r="F28" s="35">
-        <v>43</v>
-      </c>
-      <c r="G28" s="35">
-        <v>6</v>
-      </c>
-      <c r="H28" s="35">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35">
-        <v>58</v>
-      </c>
-      <c r="E29" s="35">
-        <v>0</v>
-      </c>
-      <c r="F29" s="35">
-        <v>52</v>
-      </c>
-      <c r="G29" s="35">
-        <v>6</v>
-      </c>
-      <c r="H29" s="35">
-        <v>1E+30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="12.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36">
-        <v>15</v>
-      </c>
-      <c r="E30" s="36">
-        <v>195</v>
-      </c>
-      <c r="F30" s="36">
-        <v>15</v>
-      </c>
-      <c r="G30" s="36">
-        <v>1E+30</v>
-      </c>
-      <c r="H30" s="36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K18"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="2.28515625" customWidth="1"/>
-    <col min="3" max="3" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D5" s="1">
-        <v>170</v>
-      </c>
-      <c r="E5" s="1">
-        <v>160</v>
-      </c>
-      <c r="F5" s="1">
-        <v>175</v>
-      </c>
-      <c r="G5" s="1">
-        <v>180</v>
-      </c>
-      <c r="H5" s="1">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7">
-        <f t="shared" ref="I7:I16" si="0">SUMPRODUCT(D7:H7,AgentsPerShift)</f>
-        <v>48</v>
-      </c>
-      <c r="J7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="J8" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="J9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>118</v>
-      </c>
-      <c r="J10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="J11" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="J12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="J13" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>8</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="J14" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="J15" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="J16" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D18" s="28">
-        <v>48</v>
-      </c>
-      <c r="E18" s="28">
-        <v>31</v>
-      </c>
-      <c r="F18" s="28">
-        <v>39</v>
-      </c>
-      <c r="G18" s="28">
-        <v>43</v>
-      </c>
-      <c r="H18" s="28">
-        <v>15</v>
-      </c>
-      <c r="K18" s="3">
-        <f>SUMPRODUCT(DailyCostPerAgent,AgentsPerShift)</f>
-        <v>30610</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>